<commit_message>
criação do dml e do dql do micromanu
</commit_message>
<xml_diff>
--- a/sprint-1-bd/exercicios/micromanu/micromanu.xlsx
+++ b/sprint-1-bd/exercicios/micromanu/micromanu.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\senai-dev-2s2019\sprint-1-bd\exercicios\micromanu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\senai-dev-2s2019\sprint-1-bd\exercicios\micromanu\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBA6366-7F17-4E27-8C2B-502D384EC4C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="micromanu" sheetId="1" r:id="rId1"/>
@@ -19,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -109,9 +105,6 @@
     <t>Entrada</t>
   </si>
   <si>
-    <t>Serial</t>
-  </si>
-  <si>
     <t>IdItem</t>
   </si>
   <si>
@@ -128,12 +121,15 @@
   </si>
   <si>
     <t>Limpeza</t>
+  </si>
+  <si>
+    <t>NumeroEquipamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,9 +244,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -258,6 +251,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,11 +570,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +586,7 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="1.7109375" customWidth="1"/>
@@ -602,23 +598,23 @@
   <sheetData>
     <row r="1" spans="2:14" ht="0.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -634,13 +630,13 @@
         <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>25</v>
@@ -759,27 +755,27 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="H8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
@@ -793,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -807,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -835,11 +831,11 @@
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">

</xml_diff>